<commit_message>
Update(Tableau-HTTP):Changer des informations sur les routes
</commit_message>
<xml_diff>
--- a/Tableau_HTTP-294.xlsx
+++ b/Tableau_HTTP-294.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa84igb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa84igb\Documents\GitHub\P_294-Passion_lecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9E1D6B-E6A6-4FEE-B3F0-974246815172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7053902C-DCC6-4083-B6D7-7EB512774CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64DD640D-AAE6-4407-BD4E-694126AE068C}"/>
+    <workbookView xWindow="29970" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{64DD640D-AAE6-4407-BD4E-694126AE068C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +566,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>